<commit_message>
Nuevas estimaciones. Falta incorporar las estimaciones de población
</commit_message>
<xml_diff>
--- a/graphs/Graph_Pobreza.xlsx
+++ b/graphs/Graph_Pobreza.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Gráficas pobreza" sheetId="2" r:id="rId1"/>
@@ -142,10 +142,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$B$3:$B$10</c:f>
+              <c:f>'Gráficas pobreza'!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1980</c:v>
                 </c:pt>
@@ -169,16 +169,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$C$3:$C$10</c:f>
+              <c:f>'Gráficas pobreza'!$C$3:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>18.600000000000001</c:v>
                 </c:pt>
@@ -198,10 +201,13 @@
                   <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -223,10 +229,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$B$3:$B$10</c:f>
+              <c:f>'Gráficas pobreza'!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1980</c:v>
                 </c:pt>
@@ -250,16 +256,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$D$3:$D$10</c:f>
+              <c:f>'Gráficas pobreza'!$D$3:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40.5</c:v>
                 </c:pt>
@@ -279,10 +288,13 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.4</c:v>
+                  <c:v>29.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28.8</c:v>
+                  <c:v>28.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,25 +304,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="70603520"/>
-        <c:axId val="70605056"/>
+        <c:axId val="75683328"/>
+        <c:axId val="75684864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70603520"/>
+        <c:axId val="75683328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70605056"/>
+        <c:crossAx val="75684864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70605056"/>
+        <c:axId val="75684864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,7 +336,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70603520"/>
+        <c:crossAx val="75683328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -342,7 +354,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -374,10 +386,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$B$3:$B$10</c:f>
+              <c:f>'Gráficas pobreza'!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1980</c:v>
                 </c:pt>
@@ -401,16 +413,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$G$3:$G$10</c:f>
+              <c:f>'Gráficas pobreza'!$G$3:$G$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>62</c:v>
                 </c:pt>
@@ -430,10 +445,13 @@
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>66</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -455,10 +473,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$B$3:$B$10</c:f>
+              <c:f>'Gráficas pobreza'!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1980</c:v>
                 </c:pt>
@@ -482,16 +500,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Gráficas pobreza'!$H$3:$H$10</c:f>
+              <c:f>'Gráficas pobreza'!$H$3:$H$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>136</c:v>
                 </c:pt>
@@ -511,10 +532,13 @@
                   <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>168</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>167</c:v>
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -524,25 +548,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="100"/>
-        <c:axId val="70622208"/>
-        <c:axId val="70632192"/>
+        <c:axId val="76034048"/>
+        <c:axId val="76035584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70622208"/>
+        <c:axId val="76034048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70632192"/>
+        <c:crossAx val="76035584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70632192"/>
+        <c:axId val="76035584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,9 +578,9 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70622208"/>
+        <c:crossAx val="76034048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -574,7 +598,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -932,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -965,10 +989,10 @@
       <c r="F3">
         <v>1980</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>62</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>136</v>
       </c>
     </row>
@@ -985,10 +1009,10 @@
       <c r="F4">
         <v>1990</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>95</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>204</v>
       </c>
     </row>
@@ -1005,10 +1029,10 @@
       <c r="F5">
         <v>1999</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>91</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>215</v>
       </c>
     </row>
@@ -1025,10 +1049,10 @@
       <c r="F6">
         <v>2002</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>99</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>225</v>
       </c>
     </row>
@@ -1045,10 +1069,10 @@
       <c r="F7">
         <v>2009</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>73</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>184</v>
       </c>
     </row>
@@ -1065,10 +1089,10 @@
       <c r="F8">
         <v>2010</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>69</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>176</v>
       </c>
     </row>
@@ -1077,19 +1101,19 @@
         <v>2011</v>
       </c>
       <c r="C9">
-        <v>11.5</v>
+        <v>11.6</v>
       </c>
       <c r="D9">
-        <v>29.4</v>
+        <v>29.6</v>
       </c>
       <c r="F9">
         <v>2011</v>
       </c>
-      <c r="G9">
-        <v>66</v>
-      </c>
-      <c r="H9">
-        <v>168</v>
+      <c r="G9" s="4">
+        <v>67</v>
+      </c>
+      <c r="H9" s="4">
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="2:11">
@@ -1097,23 +1121,40 @@
         <v>2012</v>
       </c>
       <c r="C10">
-        <v>11.4</v>
+        <v>11.3</v>
       </c>
       <c r="D10">
-        <v>28.8</v>
+        <v>28.2</v>
       </c>
       <c r="F10">
         <v>2012</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>66</v>
       </c>
-      <c r="H10">
-        <v>167</v>
+      <c r="H10" s="4">
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="H11" s="6"/>
+      <c r="B11">
+        <v>2013</v>
+      </c>
+      <c r="C11">
+        <v>11.5</v>
+      </c>
+      <c r="D11">
+        <v>27.9</v>
+      </c>
+      <c r="F11">
+        <v>2013</v>
+      </c>
+      <c r="G11" s="4">
+        <v>68</v>
+      </c>
+      <c r="H11" s="4">
+        <v>164</v>
+      </c>
       <c r="K11" s="2"/>
     </row>
   </sheetData>
@@ -1126,7 +1167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E7:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>

</xml_diff>